<commit_message>
SRV: lower consumption of electricity for DC to avoid dummies in 2018
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SRV_DC_EH.xlsx
+++ b/SuppXLS/Scen_B_SRV_DC_EH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CC6AF1-9627-4C96-B14A-8C6421C32801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A87240-202B-4F61-9545-A9C84123A115}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="integration" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    lower consumption electricity that is not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</t>
+    lower consumption of electricity not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</t>
       </text>
     </comment>
   </commentList>
@@ -468,7 +468,7 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="F15" dT="2021-04-21T11:38:55.94" personId="{350715B6-622E-4E35-B498-CB0D8CC3C58C}" id="{2070D2EC-AEEF-42E5-8008-CFEA22FBD9E3}">
-    <text>lower consumption electricity that is not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</text>
+    <text>lower consumption of electricity not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -652,11 +652,11 @@
         <v>19</v>
       </c>
       <c r="F15" s="1">
-        <v>1.073</v>
+        <v>1.075</v>
       </c>
       <c r="G15" s="1">
         <f>F15</f>
-        <v>1.073</v>
+        <v>1.075</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>13</v>

</xml_diff>